<commit_message>
leerdoelen updated and listtasks updated
</commit_message>
<xml_diff>
--- a/Leerdoelen.xlsx
+++ b/Leerdoelen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\ASP.NETCinema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{708E4AF8-6AC9-4E6E-AADA-2FA80685CEED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25AEB3F-8599-4653-A11C-82871392EA7C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11028" yWindow="1392" windowWidth="23256" windowHeight="12576" xr2:uid="{FB29B554-5E4E-402A-B9D0-5D17CD7A78B1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{FB29B554-5E4E-402A-B9D0-5D17CD7A78B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Css en html</t>
   </si>
@@ -115,16 +115,38 @@
   </si>
   <si>
     <t>Ex handeling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zit er in = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">zit er niet in = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">twijfel = </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,12 +190,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,7 +515,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,6 +556,10 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -540,14 +568,20 @@
       <c r="B3" s="1"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
+      <c r="I4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -574,7 +608,7 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -622,13 +656,13 @@
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">

</xml_diff>

<commit_message>
added more stored pro for screening and also updated todo
</commit_message>
<xml_diff>
--- a/Leerdoelen.xlsx
+++ b/Leerdoelen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\ASP.NETCinema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25AEB3F-8599-4653-A11C-82871392EA7C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B874FC-DF33-4E03-94C8-6087B43AEB06}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{FB29B554-5E4E-402A-B9D0-5D17CD7A78B1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB29B554-5E4E-402A-B9D0-5D17CD7A78B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +177,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -190,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -198,6 +204,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,7 +522,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,7 +711,7 @@
       <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>